<commit_message>
create template files new from scratch: unsupported openpyxl-formatting is gone
</commit_message>
<xml_diff>
--- a/docs/assets/data_model_templates/rosetta (rosetta)/resources.xlsx
+++ b/docs/assets/data_model_templates/rosetta (rosetta)/resources.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/dsp-tools/docs/assets/data_model_templates/rosetta (rosetta)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F3D71C5-609C-BA4D-8E27-4B3F9D8B0271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B79F83-2120-8340-B910-2475AD030425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{21CE00AF-D0D3-C346-89EF-6D534C639BCD}"/>
+    <workbookView xWindow="4060" yWindow="3160" windowWidth="27240" windowHeight="16440" xr2:uid="{D65EA91E-614D-7C4A-992B-E2BD6A7FAEF1}"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Image2D" sheetId="5" r:id="rId5"/>
     <sheet name="Institution" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,14 +43,14 @@
     <author>Johannes Nussbaum</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{9BF41655-EE88-6E47-947A-B4B276FB1952}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{DF181FC8-0DC5-664C-AD4D-1109FAFF6103}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">mandatory
 </t>
@@ -59,8 +59,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -69,31 +69,31 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t>Unique identifier for the resource class</t>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t>The unique identifier of the property</t>
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{59376DB9-36A1-8940-88B0-D2846912D0DF}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{50221DAF-6CD4-5C47-B4BD-072B40670CC0}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">one language mandatory
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">mandatory
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -102,21 +102,62 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t>Label of the resource class that will be displayed in DSP-APP. Should be rather short.</t>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Indicates how often the property may occur. The possible values are: 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - 1: exactly once (mandatory one value and only one)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - 0-1: The value may be omitted, but can occur only once.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - 1-n: At least one value must be present, but multiple values may be present.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - 0-n: The value may be omitted, but may also occur multiple times.
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{2C75FD9F-804B-5A45-B4B2-5E8D8117507C}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{1D54D9E1-4AB3-DF4F-B8B9-7C5B4CEC230F}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">optional
 </t>
@@ -125,8 +166,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -135,31 +176,18 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t>Description of the resource class. Can be longer than the label.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{872BF941-ED66-5347-9A5A-6BAF8A6386E0}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">mandatory
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">By default, DSP-APP displays the properties in the order how they are listed in the Excel sheet. If you prefer another order, you can make a numbering in this column.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -168,50 +196,10 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">The type of this resource class, i.e. the base resource class(es) that this resource class is derived from.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">Must be one of the values listed in the documentation. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">If more than one: separated by commas. </t>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Example: You order the propnames alphabetically in the Excel, but they should be displayed in another order in DSP-APP.</t>
         </r>
       </text>
     </comment>
@@ -225,14 +213,14 @@
     <author>Johannes Nussbaum</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{8ADC0847-6720-0B4E-A971-C3C21D242C61}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{C3EE7E7D-F573-6F4B-A857-874B79DDE039}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">mandatory
 </t>
@@ -241,8 +229,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -251,21 +239,21 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t>The unique identifier of the property</t>
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{E6BE20A6-D9DB-D544-81C5-02047AF8759B}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{EC3D802A-30E8-B94C-B0F4-BA3CF29071EA}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">mandatory
 </t>
@@ -274,8 +262,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -284,8 +272,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Indicates how often the property may occur. The possible values are: 
 </t>
@@ -294,18 +282,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve"> - 1: exactly once (mandatory one value and only one)
 </t>
@@ -314,8 +292,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve"> - 0-1: The value may be omitted, but can occur only once.
 </t>
@@ -324,8 +302,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve"> - 1-n: At least one value must be present, but multiple values may be present.
 </t>
@@ -334,21 +312,22 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve"> - 0-n: The value may be omitted, but may also occur multiple times.</t>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - 0-n: The value may be omitted, but may also occur multiple times.
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{9AC558E0-149A-4640-9E33-1547B47387C3}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{6047CB04-C234-5042-BE3C-3E9CD7E92073}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">optional
 </t>
@@ -357,8 +336,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -367,8 +346,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">By default, DSP-APP displays the properties in the order how they are listed in the Excel sheet. If you prefer another order, you can make a numbering in this column.
 </t>
@@ -377,8 +356,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -387,8 +366,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t>Example: You order the propnames alphabetically in the Excel, but they should be displayed in another order in DSP-APP.</t>
         </r>
@@ -404,14 +383,14 @@
     <author>Johannes Nussbaum</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{27E0E292-2665-9747-876D-44C4A25DA95D}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{150BB78D-5AC8-934A-B8C3-F8886E829741}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">mandatory
 </t>
@@ -420,8 +399,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -430,21 +409,21 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t>The unique identifier of the property</t>
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{6E2111B5-AEEF-3B46-BA31-2B17A63AEFC0}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{310B8EA5-3347-E141-B331-FC796C242DD1}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">mandatory
 </t>
@@ -453,8 +432,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -463,8 +442,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Indicates how often the property may occur. The possible values are: 
 </t>
@@ -473,18 +452,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve"> - 1: exactly once (mandatory one value and only one)
 </t>
@@ -493,8 +462,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve"> - 0-1: The value may be omitted, but can occur only once.
 </t>
@@ -503,8 +472,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve"> - 1-n: At least one value must be present, but multiple values may be present.
 </t>
@@ -513,21 +482,22 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve"> - 0-n: The value may be omitted, but may also occur multiple times.</t>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - 0-n: The value may be omitted, but may also occur multiple times.
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{F4197A70-1CA0-3547-99AA-89718B30CD8B}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{D175B81E-C952-3949-88A2-11637EA17205}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">optional
 </t>
@@ -536,8 +506,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -546,8 +516,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">By default, DSP-APP displays the properties in the order how they are listed in the Excel sheet. If you prefer another order, you can make a numbering in this column.
 </t>
@@ -556,8 +526,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -566,8 +536,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t>Example: You order the propnames alphabetically in the Excel, but they should be displayed in another order in DSP-APP.</t>
         </r>
@@ -583,14 +553,14 @@
     <author>Johannes Nussbaum</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{786EFD58-7312-1B49-AB3C-A162318A0F0D}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{352D4F02-EB2C-854F-A0DB-0CEF70DAAE4B}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">mandatory
 </t>
@@ -599,8 +569,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -609,21 +579,21 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t>The unique identifier of the property</t>
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{91A8E107-5A96-E64D-911C-A3592B1FF654}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{5020738C-EFA5-064B-A409-41652955C013}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">mandatory
 </t>
@@ -632,8 +602,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -642,8 +612,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Indicates how often the property may occur. The possible values are: 
 </t>
@@ -652,18 +622,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve"> - 1: exactly once (mandatory one value and only one)
 </t>
@@ -672,8 +632,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve"> - 0-1: The value may be omitted, but can occur only once.
 </t>
@@ -682,8 +642,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve"> - 1-n: At least one value must be present, but multiple values may be present.
 </t>
@@ -692,21 +652,22 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve"> - 0-n: The value may be omitted, but may also occur multiple times.</t>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - 0-n: The value may be omitted, but may also occur multiple times.
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{8B59C7E6-869E-244D-A6D0-29011FB0AE1E}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{A3FE11BD-5CF9-5D4E-BB38-A16DFE1E499F}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">optional
 </t>
@@ -715,8 +676,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -725,8 +686,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">By default, DSP-APP displays the properties in the order how they are listed in the Excel sheet. If you prefer another order, you can make a numbering in this column.
 </t>
@@ -735,8 +696,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -745,8 +706,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t>Example: You order the propnames alphabetically in the Excel, but they should be displayed in another order in DSP-APP.</t>
         </r>
@@ -762,14 +723,14 @@
     <author>Johannes Nussbaum</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{F1F1EA86-E50A-FB4F-97F7-6C1AB8EFA6A8}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{0779794D-F758-BA41-8BA0-8A0C8617685A}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">mandatory
 </t>
@@ -778,8 +739,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -788,21 +749,21 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t>The unique identifier of the property</t>
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{9AC27115-B3BD-3B4B-8E59-D3DEAA7BEE61}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{7983848E-17C6-E147-B2C8-B4938A9687A4}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">mandatory
 </t>
@@ -811,8 +772,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -821,8 +782,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Indicates how often the property may occur. The possible values are: 
 </t>
@@ -831,18 +792,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve"> - 1: exactly once (mandatory one value and only one)
 </t>
@@ -851,8 +802,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve"> - 0-1: The value may be omitted, but can occur only once.
 </t>
@@ -861,8 +812,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve"> - 1-n: At least one value must be present, but multiple values may be present.
 </t>
@@ -871,21 +822,22 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve"> - 0-n: The value may be omitted, but may also occur multiple times.</t>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - 0-n: The value may be omitted, but may also occur multiple times.
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{C72C80C3-5105-BE47-A05C-ABA0A837FC97}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{0D61626F-1174-AA41-ACCC-9E052F042037}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">optional
 </t>
@@ -894,8 +846,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -904,8 +856,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">By default, DSP-APP displays the properties in the order how they are listed in the Excel sheet. If you prefer another order, you can make a numbering in this column.
 </t>
@@ -914,8 +866,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -924,187 +876,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t>Example: You order the propnames alphabetically in the Excel, but they should be displayed in another order in DSP-APP.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Johannes Nussbaum</author>
-  </authors>
-  <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{C8654519-BB1C-CF4D-BC0A-6B2D1FD5724C}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">mandatory
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>The unique identifier of the property</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{E49E0A53-84D8-B24C-B03B-FD2382DB114D}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">mandatory
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">Indicates how often the property may occur. The possible values are: 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve"> - 1: exactly once (mandatory one value and only one)
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve"> - 0-1: The value may be omitted, but can occur only once.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve"> - 1-n: At least one value must be present, but multiple values may be present.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve"> - 0-n: The value may be omitted, but may also occur multiple times.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{21DD3828-047D-8548-939A-9EFABB5BBA21}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">optional
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">By default, DSP-APP displays the properties in the order how they are listed in the Excel sheet. If you prefer another order, you can make a numbering in this column.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
           </rPr>
           <t>Example: You order the propnames alphabetically in the Excel, but they should be displayed in another order in DSP-APP.</t>
         </r>
@@ -1120,6 +893,21 @@
     <t>name</t>
   </si>
   <si>
+    <t>label_en</t>
+  </si>
+  <si>
+    <t>label_de</t>
+  </si>
+  <si>
+    <t>label_fr</t>
+  </si>
+  <si>
+    <t>label_it</t>
+  </si>
+  <si>
+    <t>label_rm</t>
+  </si>
+  <si>
     <t>comment_en</t>
   </si>
   <si>
@@ -1135,6 +923,9 @@
     <t>comment_rm</t>
   </si>
   <si>
+    <t>super</t>
+  </si>
+  <si>
     <t>Object</t>
   </si>
   <si>
@@ -1183,6 +974,9 @@
     <t>Cardinality</t>
   </si>
   <si>
+    <t>gui_order</t>
+  </si>
+  <si>
     <t>hasImage</t>
   </si>
   <si>
@@ -1280,34 +1074,13 @@
   </si>
   <si>
     <t>linkstoRegion</t>
-  </si>
-  <si>
-    <t>label_en</t>
-  </si>
-  <si>
-    <t>label_de</t>
-  </si>
-  <si>
-    <t>label_fr</t>
-  </si>
-  <si>
-    <t>label_it</t>
-  </si>
-  <si>
-    <t>label_rm</t>
-  </si>
-  <si>
-    <t>gui_order</t>
-  </si>
-  <si>
-    <t>super</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1343,14 +1116,8 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="34"/>
+      <name val="+mn-lt"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1376,8 +1143,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1692,363 +1459,362 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6F0D3C5-BC1D-CB48-9C97-E30EC452F5BC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED459903-45FA-E349-9404-7AA844FE5625}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
+    <col min="1" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:12" s="2" customFormat="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="L2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="L3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="L4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" t="s">
         <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="L5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L6" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="name_2" xr:uid="{16E503F4-438C-A74B-814E-052C4E388BF7}"/>
-    <hyperlink ref="B1" r:id="rId2" location="labels_1" xr:uid="{FF98CB32-3B58-DE45-961F-426E66536930}"/>
-    <hyperlink ref="G1" r:id="rId3" location="comments_1" xr:uid="{A7185ED7-24ED-564B-A42A-A91CC8121D37}"/>
-    <hyperlink ref="L1" r:id="rId4" location="super_1" display="type" xr:uid="{A0AB7618-2721-6F4A-A4AC-1D456D3BFC9B}"/>
+    <hyperlink ref="A1" r:id="rId1" location="resource-name" xr:uid="{5211743E-9BD4-B04F-8E92-ECCFE51899F7}"/>
+    <hyperlink ref="B1" r:id="rId2" location="resource-labels" xr:uid="{AA4EF149-9BE9-4C42-839B-D7970F15E35F}"/>
+    <hyperlink ref="G1" r:id="rId3" location="resource-comments" xr:uid="{6C3E7B11-6E7C-DB45-8B4F-57249FBA5270}"/>
+    <hyperlink ref="L1" r:id="rId4" location="resource-super" xr:uid="{DE647869-BC1D-E74C-856F-D0A8E910012B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FE0CE73-59FD-ED4F-A98E-E325E8F2B2B8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BFF565D-812B-644B-8CC6-B2F47CD7C6A8}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView zoomScale="144" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C16">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C18">
         <v>17</v>
@@ -2056,7 +1822,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="cardinalities" xr:uid="{15B238D8-8D11-244E-AC63-58DE55235FE3}"/>
+    <hyperlink ref="A1" r:id="rId1" location="resource-cardinalities" xr:uid="{E1C98FD0-9321-6445-A1D1-1B9E5C178BCC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId2"/>
@@ -2064,136 +1830,136 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FCAE9F3-5D7E-BD4B-872F-A02BAD88F7FD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4500F83-7A6D-4142-9F07-D48EC702D432}">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
         <v>41</v>
       </c>
-      <c r="B2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
         <v>45</v>
       </c>
-      <c r="B6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>38</v>
-      </c>
       <c r="B13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="cardinalities" xr:uid="{8B9472A9-C5C7-3F42-87E0-7B42D57B1927}"/>
+    <hyperlink ref="A1" r:id="rId1" location="resource-cardinalities" xr:uid="{4FF97F19-FC9F-C24A-8E05-543AB1CDFB1B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId2"/>
@@ -2201,64 +1967,64 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A28BDDB-03FE-BF4D-939B-0B6C9B99E498}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEB53F0D-8700-8343-9A8B-FFFE95431F90}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="cardinalities" xr:uid="{0872DD1E-97EA-BE43-BFC0-76AE9286A430}"/>
+    <hyperlink ref="A1" r:id="rId1" location="resource-cardinalities" xr:uid="{7CE49DDD-198B-4047-A685-EE30D347A558}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId2"/>
@@ -2266,104 +2032,104 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{055036C3-9294-4345-9014-FBDAD87C450C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFDF0782-2125-2444-BDF4-F61FF62ECA9A}">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="cardinalities" xr:uid="{68BB1E38-978A-E743-89CF-51E9FF60A907}"/>
+    <hyperlink ref="A1" r:id="rId1" location="resource-cardinalities" xr:uid="{0570E52C-37AE-C240-BDA7-B87C8DB911E4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId2"/>
@@ -2371,64 +2137,64 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{762268FB-1B16-8D4D-A8DA-03511DF12088}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F09CD1-88AB-E444-B89C-4D3D0FC1A6D4}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="cardinalities" xr:uid="{B345A3DE-3A3C-0445-96ED-A7F54E74CD8B}"/>
+    <hyperlink ref="A1" r:id="rId1" location="resource-cardinalities" xr:uid="{3D9A8C68-8504-E747-9402-9AAAA63A9D24}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
feat(excel2json): add support for gui_order, make templates better understandable (DEV-1711) (#293)
</commit_message>
<xml_diff>
--- a/docs/assets/data_model_templates/rosetta (rosetta)/resources.xlsx
+++ b/docs/assets/data_model_templates/rosetta (rosetta)/resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nusjoh00-adm/Desktop/dsp-tools/docs/assets/data_model_templates/rosetta (rosetta)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0028FA-7D6F-504F-AA55-B56A17E13E62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B79F83-2120-8340-B910-2475AD030425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="1640" windowWidth="26160" windowHeight="15560" xr2:uid="{21CE00AF-D0D3-C346-89EF-6D534C639BCD}"/>
+    <workbookView xWindow="4060" yWindow="3160" windowWidth="27240" windowHeight="16440" xr2:uid="{D65EA91E-614D-7C4A-992B-E2BD6A7FAEF1}"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Image2D" sheetId="5" r:id="rId5"/>
     <sheet name="Institution" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,25 +37,875 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Johannes Nussbaum</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{DF181FC8-0DC5-664C-AD4D-1109FAFF6103}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">mandatory
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t>The unique identifier of the property</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{50221DAF-6CD4-5C47-B4BD-072B40670CC0}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">mandatory
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Indicates how often the property may occur. The possible values are: 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - 1: exactly once (mandatory one value and only one)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - 0-1: The value may be omitted, but can occur only once.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - 1-n: At least one value must be present, but multiple values may be present.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - 0-n: The value may be omitted, but may also occur multiple times.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{1D54D9E1-4AB3-DF4F-B8B9-7C5B4CEC230F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">optional
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">By default, DSP-APP displays the properties in the order how they are listed in the Excel sheet. If you prefer another order, you can make a numbering in this column.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Example: You order the propnames alphabetically in the Excel, but they should be displayed in another order in DSP-APP.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Johannes Nussbaum</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{C3EE7E7D-F573-6F4B-A857-874B79DDE039}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">mandatory
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t>The unique identifier of the property</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{EC3D802A-30E8-B94C-B0F4-BA3CF29071EA}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">mandatory
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Indicates how often the property may occur. The possible values are: 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - 1: exactly once (mandatory one value and only one)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - 0-1: The value may be omitted, but can occur only once.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - 1-n: At least one value must be present, but multiple values may be present.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - 0-n: The value may be omitted, but may also occur multiple times.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{6047CB04-C234-5042-BE3C-3E9CD7E92073}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">optional
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">By default, DSP-APP displays the properties in the order how they are listed in the Excel sheet. If you prefer another order, you can make a numbering in this column.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Example: You order the propnames alphabetically in the Excel, but they should be displayed in another order in DSP-APP.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Johannes Nussbaum</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{150BB78D-5AC8-934A-B8C3-F8886E829741}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">mandatory
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t>The unique identifier of the property</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{310B8EA5-3347-E141-B331-FC796C242DD1}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">mandatory
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Indicates how often the property may occur. The possible values are: 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - 1: exactly once (mandatory one value and only one)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - 0-1: The value may be omitted, but can occur only once.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - 1-n: At least one value must be present, but multiple values may be present.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - 0-n: The value may be omitted, but may also occur multiple times.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{D175B81E-C952-3949-88A2-11637EA17205}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">optional
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">By default, DSP-APP displays the properties in the order how they are listed in the Excel sheet. If you prefer another order, you can make a numbering in this column.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Example: You order the propnames alphabetically in the Excel, but they should be displayed in another order in DSP-APP.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Johannes Nussbaum</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{352D4F02-EB2C-854F-A0DB-0CEF70DAAE4B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">mandatory
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t>The unique identifier of the property</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{5020738C-EFA5-064B-A409-41652955C013}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">mandatory
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Indicates how often the property may occur. The possible values are: 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - 1: exactly once (mandatory one value and only one)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - 0-1: The value may be omitted, but can occur only once.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - 1-n: At least one value must be present, but multiple values may be present.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - 0-n: The value may be omitted, but may also occur multiple times.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{A3FE11BD-5CF9-5D4E-BB38-A16DFE1E499F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">optional
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">By default, DSP-APP displays the properties in the order how they are listed in the Excel sheet. If you prefer another order, you can make a numbering in this column.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Example: You order the propnames alphabetically in the Excel, but they should be displayed in another order in DSP-APP.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Johannes Nussbaum</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{0779794D-F758-BA41-8BA0-8A0C8617685A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">mandatory
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t>The unique identifier of the property</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{7983848E-17C6-E147-B2C8-B4938A9687A4}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">mandatory
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Indicates how often the property may occur. The possible values are: 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - 1: exactly once (mandatory one value and only one)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - 0-1: The value may be omitted, but can occur only once.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - 1-n: At least one value must be present, but multiple values may be present.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - 0-n: The value may be omitted, but may also occur multiple times.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{0D61626F-1174-AA41-ACCC-9E052F042037}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">optional
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">By default, DSP-APP displays the properties in the order how they are listed in the Excel sheet. If you prefer another order, you can make a numbering in this column.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Example: You order the propnames alphabetically in the Excel, but they should be displayed in another order in DSP-APP.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="62">
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>en</t>
-  </si>
-  <si>
-    <t>de</t>
-  </si>
-  <si>
-    <t>fr</t>
-  </si>
-  <si>
-    <t>it</t>
-  </si>
-  <si>
-    <t>rm</t>
+    <t>label_en</t>
+  </si>
+  <si>
+    <t>label_de</t>
+  </si>
+  <si>
+    <t>label_fr</t>
+  </si>
+  <si>
+    <t>label_it</t>
+  </si>
+  <si>
+    <t>label_rm</t>
   </si>
   <si>
     <t>comment_en</t>
@@ -122,6 +972,9 @@
   </si>
   <si>
     <t>Cardinality</t>
+  </si>
+  <si>
+    <t>gui_order</t>
   </si>
   <si>
     <t>hasImage</t>
@@ -227,7 +1080,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -242,6 +1095,29 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="+mn-lt"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -261,14 +1137,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -580,61 +1459,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6F0D3C5-BC1D-CB48-9C97-E30EC452F5BC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED459903-45FA-E349-9404-7AA844FE5625}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
+    <col min="1" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -651,7 +1531,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -668,7 +1548,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -685,7 +1565,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -702,7 +1582,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -720,512 +1600,603 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" location="resource-name" xr:uid="{5211743E-9BD4-B04F-8E92-ECCFE51899F7}"/>
+    <hyperlink ref="B1" r:id="rId2" location="resource-labels" xr:uid="{AA4EF149-9BE9-4C42-839B-D7970F15E35F}"/>
+    <hyperlink ref="G1" r:id="rId3" location="resource-comments" xr:uid="{6C3E7B11-6E7C-DB45-8B4F-57249FBA5270}"/>
+    <hyperlink ref="L1" r:id="rId4" location="resource-super" xr:uid="{DE647869-BC1D-E74C-856F-D0A8E910012B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FE0CE73-59FD-ED4F-A98E-E325E8F2B2B8}">
-  <dimension ref="A1:B18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BFF565D-812B-644B-8CC6-B2F47CD7C6A8}">
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
         <v>30</v>
       </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
         <v>37</v>
       </c>
-      <c r="B9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="C14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="C15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="C16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="C17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="C18">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" location="resource-cardinalities" xr:uid="{E1C98FD0-9321-6445-A1D1-1B9E5C178BCC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FCAE9F3-5D7E-BD4B-872F-A02BAD88F7FD}">
-  <dimension ref="A1:B14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4500F83-7A6D-4142-9F07-D48EC702D432}">
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
         <v>37</v>
       </c>
-      <c r="B9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" location="resource-cardinalities" xr:uid="{4FF97F19-FC9F-C24A-8E05-543AB1CDFB1B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A28BDDB-03FE-BF4D-939B-0B6C9B99E498}">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEB53F0D-8700-8343-9A8B-FFFE95431F90}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" location="resource-cardinalities" xr:uid="{7CE49DDD-198B-4047-A685-EE30D347A558}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{055036C3-9294-4345-9014-FBDAD87C450C}">
-  <dimension ref="A1:B10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFDF0782-2125-2444-BDF4-F61FF62ECA9A}">
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" location="resource-cardinalities" xr:uid="{0570E52C-37AE-C240-BDA7-B87C8DB911E4}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{762268FB-1B16-8D4D-A8DA-03511DF12088}">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F09CD1-88AB-E444-B89C-4D3D0FC1A6D4}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" location="resource-cardinalities" xr:uid="{3D9A8C68-8504-E747-9402-9AAAA63A9D24}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix(excel2json): add missing comments in the resources template (DEV-1765) #303
</commit_message>
<xml_diff>
--- a/docs/assets/data_model_templates/rosetta (rosetta)/resources.xlsx
+++ b/docs/assets/data_model_templates/rosetta (rosetta)/resources.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/dsp-tools/docs/assets/data_model_templates/rosetta (rosetta)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B79F83-2120-8340-B910-2475AD030425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C00672D-AAE4-654A-B8F3-BE3045DB89F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4060" yWindow="3160" windowWidth="27240" windowHeight="16440" xr2:uid="{D65EA91E-614D-7C4A-992B-E2BD6A7FAEF1}"/>
   </bookViews>
@@ -43,14 +43,14 @@
     <author>Johannes Nussbaum</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{DF181FC8-0DC5-664C-AD4D-1109FAFF6103}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{E89493F0-EE89-2143-8A32-3A8667F7809D}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="+mn-lt"/>
-            <charset val="1"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">mandatory
 </t>
@@ -59,105 +59,64 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="+mn-lt"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="+mn-lt"/>
-            <charset val="1"/>
-          </rPr>
-          <t>The unique identifier of the property</t>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Unique identifier for the resource class</t>
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{50221DAF-6CD4-5C47-B4BD-072B40670CC0}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{C9356C15-819C-B446-A19E-3508C45688E6}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="+mn-lt"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">mandatory
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="+mn-lt"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="+mn-lt"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Indicates how often the property may occur. The possible values are: 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="+mn-lt"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve"> - 1: exactly once (mandatory one value and only one)
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="+mn-lt"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve"> - 0-1: The value may be omitted, but can occur only once.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="+mn-lt"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve"> - 1-n: At least one value must be present, but multiple values may be present.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="+mn-lt"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve"> - 0-n: The value may be omitted, but may also occur multiple times.
-</t>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">one language mandatory
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Label of the resource class that will be displayed in DSP-APP. Should be rather short.</t>
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{1D54D9E1-4AB3-DF4F-B8B9-7C5B4CEC230F}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{CF3C06AB-030C-E349-A5B7-C6E9B0DBDFA4}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="+mn-lt"/>
-            <charset val="1"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">optional
 </t>
@@ -166,40 +125,93 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="+mn-lt"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="+mn-lt"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">By default, DSP-APP displays the properties in the order how they are listed in the Excel sheet. If you prefer another order, you can make a numbering in this column.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="+mn-lt"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="+mn-lt"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Example: You order the propnames alphabetically in the Excel, but they should be displayed in another order in DSP-APP.</t>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Description of the resource class. Can be longer than the label.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{DA8219AF-1563-F84F-B43A-186B7F0C6225}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">mandatory
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The type of this resource class, i.e. the base resource class(es) that this resource class is derived from.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Must be one of the values listed in the documentation. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">If more than one: separated by commas. </t>
         </r>
       </text>
     </comment>
@@ -213,7 +225,7 @@
     <author>Johannes Nussbaum</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{C3EE7E7D-F573-6F4B-A857-874B79DDE039}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{DF181FC8-0DC5-664C-AD4D-1109FAFF6103}">
       <text>
         <r>
           <rPr>
@@ -246,7 +258,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{EC3D802A-30E8-B94C-B0F4-BA3CF29071EA}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{50221DAF-6CD4-5C47-B4BD-072B40670CC0}">
       <text>
         <r>
           <rPr>
@@ -320,7 +332,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{6047CB04-C234-5042-BE3C-3E9CD7E92073}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{1D54D9E1-4AB3-DF4F-B8B9-7C5B4CEC230F}">
       <text>
         <r>
           <rPr>
@@ -383,7 +395,7 @@
     <author>Johannes Nussbaum</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{150BB78D-5AC8-934A-B8C3-F8886E829741}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{C3EE7E7D-F573-6F4B-A857-874B79DDE039}">
       <text>
         <r>
           <rPr>
@@ -416,7 +428,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{310B8EA5-3347-E141-B331-FC796C242DD1}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{EC3D802A-30E8-B94C-B0F4-BA3CF29071EA}">
       <text>
         <r>
           <rPr>
@@ -490,7 +502,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{D175B81E-C952-3949-88A2-11637EA17205}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{6047CB04-C234-5042-BE3C-3E9CD7E92073}">
       <text>
         <r>
           <rPr>
@@ -553,7 +565,7 @@
     <author>Johannes Nussbaum</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{352D4F02-EB2C-854F-A0DB-0CEF70DAAE4B}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{150BB78D-5AC8-934A-B8C3-F8886E829741}">
       <text>
         <r>
           <rPr>
@@ -586,7 +598,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{5020738C-EFA5-064B-A409-41652955C013}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{310B8EA5-3347-E141-B331-FC796C242DD1}">
       <text>
         <r>
           <rPr>
@@ -660,7 +672,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{A3FE11BD-5CF9-5D4E-BB38-A16DFE1E499F}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{D175B81E-C952-3949-88A2-11637EA17205}">
       <text>
         <r>
           <rPr>
@@ -723,6 +735,176 @@
     <author>Johannes Nussbaum</author>
   </authors>
   <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{352D4F02-EB2C-854F-A0DB-0CEF70DAAE4B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">mandatory
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t>The unique identifier of the property</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{5020738C-EFA5-064B-A409-41652955C013}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">mandatory
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Indicates how often the property may occur. The possible values are: 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - 1: exactly once (mandatory one value and only one)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - 0-1: The value may be omitted, but can occur only once.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - 1-n: At least one value must be present, but multiple values may be present.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - 0-n: The value may be omitted, but may also occur multiple times.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{A3FE11BD-5CF9-5D4E-BB38-A16DFE1E499F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">optional
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">By default, DSP-APP displays the properties in the order how they are listed in the Excel sheet. If you prefer another order, you can make a numbering in this column.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Example: You order the propnames alphabetically in the Excel, but they should be displayed in another order in DSP-APP.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Johannes Nussbaum</author>
+  </authors>
+  <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{0779794D-F758-BA41-8BA0-8A0C8617685A}">
       <text>
         <r>
@@ -1080,7 +1262,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1118,6 +1300,12 @@
       <color rgb="FF000000"/>
       <name val="+mn-lt"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1459,11 +1647,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED459903-45FA-E349-9404-7AA844FE5625}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED459903-45FA-E349-9404-7AA844FE5625}">
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1607,6 +1795,7 @@
     <hyperlink ref="L1" r:id="rId4" location="resource-super" xr:uid="{DE647869-BC1D-E74C-856F-D0A8E910012B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>